<commit_message>
Improve Inverse + Added Global Speed Ctrl
</commit_message>
<xml_diff>
--- a/Breakdown/Excel/Arm Info.xlsx
+++ b/Breakdown/Excel/Arm Info.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Udin\Kuliah\7. TUGAS AKHIR\Arm Manipulator\Breakdown\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828C9AA5-E8F1-4A4D-A717-1C84B02964AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA4F6B5-27FD-4A4A-8B3D-968BB66854D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{313879A8-645A-4312-965B-79C9BD650931}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{313879A8-645A-4312-965B-79C9BD650931}"/>
   </bookViews>
   <sheets>
     <sheet name="Stepper Information" sheetId="1" r:id="rId1"/>
-    <sheet name="Cable Connection" sheetId="3" r:id="rId2"/>
-    <sheet name="Kinematics Overview" sheetId="2" r:id="rId3"/>
+    <sheet name="Speed Sync Calculation" sheetId="4" r:id="rId2"/>
+    <sheet name="Cable Connection" sheetId="3" r:id="rId3"/>
+    <sheet name="Kinematics Overview" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="187">
   <si>
     <t>No</t>
   </si>
@@ -655,6 +656,30 @@
   </si>
   <si>
     <t>JOINT ANGLE LIMIT</t>
+  </si>
+  <si>
+    <t>Current
+Angle</t>
+  </si>
+  <si>
+    <t>Goal
+Angle</t>
+  </si>
+  <si>
+    <t>Delta
+Angle</t>
+  </si>
+  <si>
+    <t>Sync
+RPM</t>
+  </si>
+  <si>
+    <t>Max
+Angle</t>
+  </si>
+  <si>
+    <t>Max
+Joint RPM</t>
   </si>
 </sst>
 </file>
@@ -967,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1218,7 +1243,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2294,7 +2322,7 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2843,11 +2871,224 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7C7809-8610-4458-B9DF-C9E7209DEAE1}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="8" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="84">
+        <v>10</v>
+      </c>
+      <c r="D3" s="84">
+        <v>15</v>
+      </c>
+      <c r="E3" s="84">
+        <f>ABS(D3-C3)</f>
+        <v>5</v>
+      </c>
+      <c r="F3" s="49">
+        <v>5</v>
+      </c>
+      <c r="G3" s="85">
+        <f>MAX(E3:E8)</f>
+        <v>50</v>
+      </c>
+      <c r="H3" s="3">
+        <f>F3*(E3/G3)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="84">
+        <v>5</v>
+      </c>
+      <c r="D4" s="84">
+        <v>20</v>
+      </c>
+      <c r="E4" s="84">
+        <f t="shared" ref="E4:E8" si="0">ABS(D4-C4)</f>
+        <v>15</v>
+      </c>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="3">
+        <f>F3*(E4/G3)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="84">
+        <v>-10</v>
+      </c>
+      <c r="D5" s="84">
+        <v>30</v>
+      </c>
+      <c r="E5" s="84">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="3">
+        <f>F3*(E5/G3)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="84">
+        <v>20</v>
+      </c>
+      <c r="D6" s="84">
+        <v>40</v>
+      </c>
+      <c r="E6" s="84">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="3">
+        <f>F3*(E6/G3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="84">
+        <v>-15</v>
+      </c>
+      <c r="D7" s="84">
+        <v>35</v>
+      </c>
+      <c r="E7" s="84">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="3">
+        <f>F3*(E7/G3)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="84">
+        <v>5</v>
+      </c>
+      <c r="D8" s="84">
+        <v>-10</v>
+      </c>
+      <c r="E8" s="84">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="3">
+        <f>F3*(E8/G3)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="G3:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="H4" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119A60BB-A318-41A1-9642-6D3A473AEA27}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3529,12 +3770,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF990D27-4B97-4251-AD4B-2BBC3FAFA5B8}">
   <dimension ref="A1:AT83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z78" sqref="Z78"/>
+    <sheetView zoomScale="38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -3830,7 +4071,7 @@
         <v>43</v>
       </c>
       <c r="X6" s="6">
-        <f t="shared" ref="X6:X11" si="0">P6</f>
+        <f>P6</f>
         <v>598.5</v>
       </c>
       <c r="Y6" s="49" t="s">
@@ -3899,7 +4140,7 @@
         <v>44</v>
       </c>
       <c r="X7" s="6">
-        <f t="shared" si="0"/>
+        <f>P7</f>
         <v>3.369158250998705E-15</v>
       </c>
       <c r="Y7" s="54"/>
@@ -3966,7 +4207,6 @@
         <v>45</v>
       </c>
       <c r="X8" s="6">
-        <f t="shared" si="0"/>
         <v>776</v>
       </c>
       <c r="Y8" s="50"/>
@@ -3993,7 +4233,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="6">
-        <f t="shared" ref="D9:D11" si="1">RADIANS(C9)</f>
+        <f t="shared" ref="D9:D11" si="0">RADIANS(C9)</f>
         <v>0</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -4039,7 +4279,7 @@
         <v>47</v>
       </c>
       <c r="X9" s="6">
-        <f t="shared" si="0"/>
+        <f>P9</f>
         <v>180</v>
       </c>
       <c r="Y9" s="6">
@@ -4115,11 +4355,11 @@
         <v>48</v>
       </c>
       <c r="X10" s="6">
-        <f t="shared" si="0"/>
+        <f>P10</f>
         <v>7.0195835743237771E-15</v>
       </c>
       <c r="Y10" s="6">
-        <f t="shared" ref="Y10:Y11" si="2">RADIANS(X10)</f>
+        <f t="shared" ref="Y10:Y11" si="1">RADIANS(X10)</f>
         <v>1.22514845490862E-16</v>
       </c>
       <c r="AA10" s="8" t="s">
@@ -4145,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -4191,11 +4431,11 @@
         <v>46</v>
       </c>
       <c r="X11" s="6">
-        <f t="shared" si="0"/>
+        <f>P11</f>
         <v>180</v>
       </c>
       <c r="Y11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.1415926535897931</v>
       </c>
       <c r="AA11" s="8" t="s">
@@ -4348,19 +4588,19 @@
       </c>
       <c r="AA16" s="17"/>
       <c r="AB16" s="6">
-        <f t="shared" ref="AB16:AE19" si="3">F32</f>
+        <f t="shared" ref="AB16:AE19" si="2">F32</f>
         <v>1</v>
       </c>
       <c r="AC16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF16" s="17"/>
@@ -4445,19 +4685,19 @@
       </c>
       <c r="AA17" s="17"/>
       <c r="AB17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF17" s="17"/>
@@ -4540,19 +4780,19 @@
       </c>
       <c r="AA18" s="17"/>
       <c r="AB18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AE18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF18" s="17"/>
@@ -4625,19 +4865,19 @@
       </c>
       <c r="AA19" s="17"/>
       <c r="AB19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AF19" s="17"/>
@@ -6456,7 +6696,7 @@
         <v>108</v>
       </c>
       <c r="B60" s="6">
-        <f t="shared" ref="B60:B62" si="4">M32</f>
+        <f t="shared" ref="B60:B62" si="3">M32</f>
         <v>0</v>
       </c>
       <c r="C60" s="76" t="s">
@@ -6522,7 +6762,7 @@
     <row r="61" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A61" s="77"/>
       <c r="B61" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C61" s="77"/>
@@ -6542,7 +6782,7 @@
         <v>585</v>
       </c>
       <c r="I61" s="25">
-        <f t="shared" ref="I61:I69" si="5">B60</f>
+        <f t="shared" ref="I61:I69" si="4">B60</f>
         <v>0</v>
       </c>
       <c r="K61" s="6">
@@ -6578,7 +6818,7 @@
     <row r="62" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A62" s="78"/>
       <c r="B62" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="C62" s="78"/>
@@ -6596,7 +6836,7 @@
         <v>3.5223018078622825E-14</v>
       </c>
       <c r="I62" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K62" s="6">
@@ -6636,8 +6876,8 @@
       <c r="AA62" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AB62" s="84" t="str">
-        <f>IF(OR(AB6&gt;Y62, AB6&lt;X62), "L", "N")</f>
+      <c r="AB62" s="3" t="str">
+        <f t="shared" ref="AB62:AB67" si="5">IF(OR(AB6&gt;Y62, AB6&lt;X62), "L", "N")</f>
         <v>N</v>
       </c>
     </row>
@@ -6666,7 +6906,7 @@
         <v>-575</v>
       </c>
       <c r="I63" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="K63" s="6">
@@ -6706,8 +6946,8 @@
       <c r="AA63" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AB63" s="84" t="str">
-        <f>IF(OR(AB7&gt;Y63, AB7&lt;X63), "L", "N")</f>
+      <c r="AB63" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
     </row>
@@ -6734,7 +6974,7 @@
         <v>-65</v>
       </c>
       <c r="I64" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K64" s="6">
@@ -6774,8 +7014,8 @@
       <c r="AA64" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AB64" s="84" t="str">
-        <f>IF(OR(AB8&gt;Y64, AB8&lt;X64), "L", "N")</f>
+      <c r="AB64" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
     </row>
@@ -6800,7 +7040,7 @@
         <v>3.5223018078622825E-14</v>
       </c>
       <c r="I65" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K65" s="6">
@@ -6840,8 +7080,8 @@
       <c r="AA65" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AB65" s="84" t="str">
-        <f>IF(OR(AB9&gt;Y65, AB9&lt;X65), "L", "N")</f>
+      <c r="AB65" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
     </row>
@@ -6870,7 +7110,7 @@
         <v>-575</v>
       </c>
       <c r="I66" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="V66" s="23"/>
@@ -6886,8 +7126,8 @@
       <c r="AA66" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AB66" s="84" t="str">
-        <f>IF(OR(AB10&gt;Y66, AB10&lt;X66), "L", "N")</f>
+      <c r="AB66" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
     </row>
@@ -6914,7 +7154,7 @@
         <v>-3.9817324784530174E-15</v>
       </c>
       <c r="I67" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V67" s="23"/>
@@ -6930,8 +7170,8 @@
       <c r="AA67" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AB67" s="84" t="str">
-        <f>IF(OR(AB11&gt;Y67, AB11&lt;X67), "L", "N")</f>
+      <c r="AB67" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
     </row>
@@ -6956,7 +7196,7 @@
         <v>65.000000000000028</v>
       </c>
       <c r="I68" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="M68" s="81" t="s">
@@ -6976,7 +7216,7 @@
         <v>7.9634649569060301E-15</v>
       </c>
       <c r="I69" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="M69" s="27" t="str">

</xml_diff>